<commit_message>
adiciona crédito das imagens na planilha
</commit_message>
<xml_diff>
--- a/Lista-de-Convidados.xlsx
+++ b/Lista-de-Convidados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laísse\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laísse\Documents\GitHub\Lista-de-Casamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Convidado</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Convite Enviado?</t>
+  </si>
+  <si>
+    <t>Imagem Superior</t>
+  </si>
+  <si>
+    <t>Imagem Lateral</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -526,6 +532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1083,9 +1090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M1128"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8149,7 +8154,7 @@
   <dimension ref="C2:P14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8269,12 +8274,22 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="E13" s="38" t="s">
+        <v>47</v>
+      </c>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="E14" s="38" t="s">
+        <v>48</v>
+      </c>
       <c r="F14" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E13" r:id="rId1"/>
+    <hyperlink ref="E14" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>